<commit_message>
add design for pos loan
</commit_message>
<xml_diff>
--- a/homecredit/vardesign/var_credit_card_balance.xlsx
+++ b/homecredit/vardesign/var_credit_card_balance.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="179">
   <si>
     <t>Table</t>
   </si>
@@ -556,6 +556,15 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>rule</t>
+  </si>
+  <si>
+    <t>rules</t>
+  </si>
+  <si>
+    <t>conmethod</t>
   </si>
 </sst>
 </file>
@@ -602,7 +611,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +621,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,7 +677,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -667,6 +688,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1251,13 +1276,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:W68"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,7 +1294,7 @@
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>71</v>
       </c>
@@ -1277,7 +1302,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -1298,7 +1323,7 @@
       </c>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>57</v>
       </c>
@@ -1319,7 +1344,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>
@@ -1343,7 +1368,7 @@
         <v>161</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>162</v>
@@ -1351,8 +1376,18 @@
       <c r="L4" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
@@ -1383,8 +1418,48 @@
       <c r="M5" s="6" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="13" t="str">
+        <f>CONCATENATE("'",H$4,"':",IF(ISBLANK(H5),"None",CONCATENATE("'",H5,"'")))</f>
+        <v>'cols':'SK_DPD'</v>
+      </c>
+      <c r="O5" s="13" t="str">
+        <f t="shared" ref="O5:R5" si="0">CONCATENATE("'",I$4,"':",IF(ISBLANK(I5),"None",CONCATENATE("'",I5,"'")))</f>
+        <v>'exmethod':None</v>
+      </c>
+      <c r="P5" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>'conmethod':'D'</v>
+      </c>
+      <c r="Q5" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>'exobj':None</v>
+      </c>
+      <c r="R5" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>'conobj':'CAC'</v>
+      </c>
+      <c r="S5" s="11" t="str">
+        <f>N5</f>
+        <v>'cols':'SK_DPD'</v>
+      </c>
+      <c r="T5" s="11" t="str">
+        <f>S5&amp;","&amp;O5</f>
+        <v>'cols':'SK_DPD','exmethod':None</v>
+      </c>
+      <c r="U5" s="11" t="str">
+        <f t="shared" ref="U5:W5" si="1">T5&amp;","&amp;P5</f>
+        <v>'cols':'SK_DPD','exmethod':None,'conmethod':'D'</v>
+      </c>
+      <c r="V5" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>'cols':'SK_DPD','exmethod':None,'conmethod':'D','exobj':None</v>
+      </c>
+      <c r="W5" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>'cols':'SK_DPD','exmethod':None,'conmethod':'D','exobj':None,'conobj':'CAC'</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1412,8 +1487,48 @@
       <c r="L6" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="13" t="str">
+        <f t="shared" ref="N6:N8" si="2">CONCATENATE("'",H$4,"':",IF(ISBLANK(H6),"None",CONCATENATE("'",H6,"'")))</f>
+        <v>'cols':'AMT_CREDIT_LIMIT_ACTUAL_Q'</v>
+      </c>
+      <c r="O6" s="13" t="str">
+        <f t="shared" ref="O6:O8" si="3">CONCATENATE("'",I$4,"':",IF(ISBLANK(I6),"None",CONCATENATE("'",I6,"'")))</f>
+        <v>'exmethod':None</v>
+      </c>
+      <c r="P6" s="13" t="str">
+        <f t="shared" ref="P6:P8" si="4">CONCATENATE("'",J$4,"':",IF(ISBLANK(J6),"None",CONCATENATE("'",J6,"'")))</f>
+        <v>'conmethod':'D'</v>
+      </c>
+      <c r="Q6" s="13" t="str">
+        <f t="shared" ref="Q6:Q8" si="5">CONCATENATE("'",K$4,"':",IF(ISBLANK(K6),"None",CONCATENATE("'",K6,"'")))</f>
+        <v>'exobj':None</v>
+      </c>
+      <c r="R6" s="13" t="str">
+        <f t="shared" ref="R6:R8" si="6">CONCATENATE("'",L$4,"':",IF(ISBLANK(L6),"None",CONCATENATE("'",L6,"'")))</f>
+        <v>'conobj':'CAC'</v>
+      </c>
+      <c r="S6" s="11" t="str">
+        <f t="shared" ref="S6:S8" si="7">N6</f>
+        <v>'cols':'AMT_CREDIT_LIMIT_ACTUAL_Q'</v>
+      </c>
+      <c r="T6" s="11" t="str">
+        <f t="shared" ref="T6:T8" si="8">S6&amp;","&amp;O6</f>
+        <v>'cols':'AMT_CREDIT_LIMIT_ACTUAL_Q','exmethod':None</v>
+      </c>
+      <c r="U6" s="11" t="str">
+        <f t="shared" ref="U6:U8" si="9">T6&amp;","&amp;P6</f>
+        <v>'cols':'AMT_CREDIT_LIMIT_ACTUAL_Q','exmethod':None,'conmethod':'D'</v>
+      </c>
+      <c r="V6" s="11" t="str">
+        <f t="shared" ref="V6:V8" si="10">U6&amp;","&amp;Q6</f>
+        <v>'cols':'AMT_CREDIT_LIMIT_ACTUAL_Q','exmethod':None,'conmethod':'D','exobj':None</v>
+      </c>
+      <c r="W6" s="11" t="str">
+        <f t="shared" ref="W6:W8" si="11">V6&amp;","&amp;R6</f>
+        <v>'cols':'AMT_CREDIT_LIMIT_ACTUAL_Q','exmethod':None,'conmethod':'D','exobj':None,'conobj':'CAC'</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1442,8 +1557,48 @@
       <c r="M7" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>'cols':'timecol'</v>
+      </c>
+      <c r="O7" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>'exmethod':None</v>
+      </c>
+      <c r="P7" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>'conmethod':None</v>
+      </c>
+      <c r="Q7" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>'exobj':'MBA'</v>
+      </c>
+      <c r="R7" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>'conobj':None</v>
+      </c>
+      <c r="S7" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>'cols':'timecol'</v>
+      </c>
+      <c r="T7" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>'cols':'timecol','exmethod':None</v>
+      </c>
+      <c r="U7" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>'cols':'timecol','exmethod':None,'conmethod':None</v>
+      </c>
+      <c r="V7" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>'cols':'timecol','exmethod':None,'conmethod':None,'exobj':'MBA'</v>
+      </c>
+      <c r="W7" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>'cols':'timecol','exmethod':None,'conmethod':None,'exobj':'MBA','conobj':None</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>57</v>
       </c>
@@ -1472,8 +1627,48 @@
       <c r="M8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>'cols':None</v>
+      </c>
+      <c r="O8" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>'exmethod':None</v>
+      </c>
+      <c r="P8" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>'conmethod':'D'</v>
+      </c>
+      <c r="Q8" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>'exobj':None</v>
+      </c>
+      <c r="R8" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>'conobj':'CAC'</v>
+      </c>
+      <c r="S8" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>'cols':None</v>
+      </c>
+      <c r="T8" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>'cols':None,'exmethod':None</v>
+      </c>
+      <c r="U8" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>'cols':None,'exmethod':None,'conmethod':'D'</v>
+      </c>
+      <c r="V8" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>'cols':None,'exmethod':None,'conmethod':'D','exobj':None</v>
+      </c>
+      <c r="W8" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>'cols':None,'exmethod':None,'conmethod':'D','exobj':None,'conobj':'CAC'</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1491,7 +1686,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>57</v>
       </c>
@@ -1511,7 +1706,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1529,7 +1724,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1550,7 +1745,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>57</v>
       </c>
@@ -1558,7 +1753,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="2" t="str">
-        <f t="shared" ref="C13:C20" si="0">B13&amp;"_Q"</f>
+        <f t="shared" ref="C13:C20" si="12">B13&amp;"_Q"</f>
         <v>AMT_CREDIT_LIMIT_ACTUAL_Q</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1569,7 +1764,7 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>57</v>
       </c>
@@ -1577,7 +1772,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>AMT_CREDIT_LIMIT_ACTUAL_Q</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1588,7 +1783,7 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1596,7 +1791,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>AMT_CREDIT_LIMIT_ACTUAL_Q</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1607,7 +1802,7 @@
       </c>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>57</v>
       </c>
@@ -1615,7 +1810,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>MONTHS_BALANCE_Q</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1634,7 +1829,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>MONTHS_BALANCE_Q</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1653,7 +1848,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>MONTHS_BALANCE_Q</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1672,7 +1867,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>MONTHS_BALANCE_Q</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1691,7 +1886,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>MONTHS_BALANCE_Q</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1729,7 +1924,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="2" t="str">
-        <f t="shared" ref="C22:C24" si="1">B22&amp;"_H"</f>
+        <f t="shared" ref="C22:C24" si="13">B22&amp;"_H"</f>
         <v>MONTHS_BALANCE_H</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1748,7 +1943,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>MONTHS_BALANCE_H</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1767,7 +1962,7 @@
         <v>10</v>
       </c>
       <c r="C24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>MONTHS_BALANCE_H</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1805,7 +2000,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="2" t="str">
-        <f t="shared" ref="C26:C30" si="2">B26&amp;"_Y"</f>
+        <f t="shared" ref="C26:C30" si="14">B26&amp;"_Y"</f>
         <v>MONTHS_BALANCE_Y</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -1824,7 +2019,7 @@
         <v>10</v>
       </c>
       <c r="C27" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>MONTHS_BALANCE_Y</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1843,7 +2038,7 @@
         <v>10</v>
       </c>
       <c r="C28" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>MONTHS_BALANCE_Y</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -1862,7 +2057,7 @@
         <v>10</v>
       </c>
       <c r="C29" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>MONTHS_BALANCE_Y</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -1881,7 +2076,7 @@
         <v>10</v>
       </c>
       <c r="C30" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>MONTHS_BALANCE_Y</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -1917,7 +2112,7 @@
         <v>41</v>
       </c>
       <c r="C32" s="2" t="str">
-        <f t="shared" ref="C32:C51" si="3">B32&amp;""</f>
+        <f t="shared" ref="C32:C51" si="15">B32&amp;""</f>
         <v>CNT_DRAWINGS_OTHER_CURRENT</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1934,7 +2129,7 @@
         <v>39</v>
       </c>
       <c r="C33" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>CNT_DRAWINGS_CURRENT</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1951,7 +2146,7 @@
         <v>15</v>
       </c>
       <c r="C34" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_CREDIT_LIMIT_ACTUAL</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -1968,7 +2163,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>CNT_DRAWINGS_POS_CURRENT</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -1985,7 +2180,7 @@
         <v>45</v>
       </c>
       <c r="C36" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>CNT_INSTALMENT_MATURE_CUM</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -2002,7 +2197,7 @@
         <v>21</v>
       </c>
       <c r="C37" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_DRAWINGS_OTHER_CURRENT</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -2019,7 +2214,7 @@
         <v>27</v>
       </c>
       <c r="C38" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_PAYMENT_CURRENT</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -2036,7 +2231,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_BALANCE</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -2053,7 +2248,7 @@
         <v>25</v>
       </c>
       <c r="C40" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_INST_MIN_REGULARITY</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -2070,7 +2265,7 @@
         <v>29</v>
       </c>
       <c r="C41" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_PAYMENT_TOTAL_CURRENT</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -2087,7 +2282,7 @@
         <v>31</v>
       </c>
       <c r="C42" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_RECEIVABLE_PRINCIPAL</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -2104,7 +2299,7 @@
         <v>49</v>
       </c>
       <c r="C43" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>SK_DPD</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -2121,7 +2316,7 @@
         <v>19</v>
       </c>
       <c r="C44" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_DRAWINGS_CURRENT</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -2138,7 +2333,7 @@
         <v>51</v>
       </c>
       <c r="C45" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>SK_DPD_DEF</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -2155,7 +2350,7 @@
         <v>35</v>
       </c>
       <c r="C46" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_TOTAL_RECEIVABLE</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -2172,7 +2367,7 @@
         <v>37</v>
       </c>
       <c r="C47" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>CNT_DRAWINGS_ATM_CURRENT</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -2189,7 +2384,7 @@
         <v>23</v>
       </c>
       <c r="C48" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_DRAWINGS_POS_CURRENT</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -2206,7 +2401,7 @@
         <v>17</v>
       </c>
       <c r="C49" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>AMT_DRAWINGS_ATM_CURRENT</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -2223,7 +2418,7 @@
         <v>70</v>
       </c>
       <c r="C50" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>bal_util</v>
       </c>
       <c r="D50" s="3" t="s">
@@ -2242,7 +2437,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">SK_ID_PREV </v>
       </c>
       <c r="D51" s="3" t="s">

</xml_diff>